<commit_message>
update to manual status column;
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_0647.xlsx
+++ b/fastqFiles/fastq_0647.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="32">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">s_6_withindex_sequence_CGCTACA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[10]</t>
   </si>
   <si>
     <t xml:space="preserve">s_6_withindex_sequence_TGGCATA.fastq.gz</t>
@@ -213,12 +216,15 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W12" activeCellId="0" sqref="W12"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="74.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="69.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,8 +625,8 @@
       <c r="H18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="0" t="n">
-        <v>10</v>
+      <c r="I18" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>19</v>

</xml_diff>